<commit_message>
Modified Clerk plan and stage audit
</commit_message>
<xml_diff>
--- a/Tools/Clerk Blank.xlsx
+++ b/Tools/Clerk Blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96892E03-9E4B-4612-9D63-0CD204EB4DDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E7ABFA-CC3F-4BD3-ACA9-C2C182CA1C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Staged Loaded Average</t>
   </si>
@@ -56,13 +56,166 @@
   </si>
   <si>
     <t>PAGER</t>
+  </si>
+  <si>
+    <t>RM-HV</t>
+  </si>
+  <si>
+    <t>DBS3-MR</t>
+  </si>
+  <si>
+    <t>DBS2-MR</t>
+  </si>
+  <si>
+    <t>DBI4-ND</t>
+  </si>
+  <si>
+    <t>STN8</t>
+  </si>
+  <si>
+    <t>JP Carts</t>
+  </si>
+  <si>
+    <t>DSN1-ND</t>
+  </si>
+  <si>
+    <t>BHX8</t>
+  </si>
+  <si>
+    <t>DBI5-MR</t>
+  </si>
+  <si>
+    <t>DWR1-MR</t>
+  </si>
+  <si>
+    <t>DEX2-ND</t>
+  </si>
+  <si>
+    <t>LCY8</t>
+  </si>
+  <si>
+    <t>LBA8</t>
+  </si>
+  <si>
+    <t>MAN8</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>DPD</t>
+  </si>
+  <si>
+    <t>BFSA</t>
+  </si>
+  <si>
+    <t>RM-H1</t>
+  </si>
+  <si>
+    <t>BRISTOL2</t>
+  </si>
+  <si>
+    <t>CARDIFF</t>
+  </si>
+  <si>
+    <t>EXETER</t>
+  </si>
+  <si>
+    <t>PLYMOUTH</t>
+  </si>
+  <si>
+    <t>SWANSEA</t>
+  </si>
+  <si>
+    <t>DRH1-ND</t>
+  </si>
+  <si>
+    <t>DSA1-ND</t>
+  </si>
+  <si>
+    <t>DNG2-ND</t>
+  </si>
+  <si>
+    <t>DBS3-SD</t>
+  </si>
+  <si>
+    <t>SXW2</t>
+  </si>
+  <si>
+    <t>DRR1-ND</t>
+  </si>
+  <si>
+    <t>DHA2-ND</t>
+  </si>
+  <si>
+    <t>DCF1-SD</t>
+  </si>
+  <si>
+    <t>DNN1-ND</t>
+  </si>
+  <si>
+    <t>DBI2-ND</t>
+  </si>
+  <si>
+    <t>DPO1-ND</t>
+  </si>
+  <si>
+    <t>DCR2-ND</t>
+  </si>
+  <si>
+    <t>DSO2-ND</t>
+  </si>
+  <si>
+    <t>DSA1-SD</t>
+  </si>
+  <si>
+    <t>DXP1-ND</t>
+  </si>
+  <si>
+    <t>DBH3-ND</t>
+  </si>
+  <si>
+    <t>DCF1-ND</t>
+  </si>
+  <si>
+    <t>DRG2-ND</t>
+  </si>
+  <si>
+    <t>DHA1-ND</t>
+  </si>
+  <si>
+    <t>SEH1</t>
+  </si>
+  <si>
+    <t>DXM2-ND</t>
+  </si>
+  <si>
+    <t>DEX2-SD</t>
+  </si>
+  <si>
+    <t>DBI7-ND</t>
+  </si>
+  <si>
+    <t>34/35</t>
+  </si>
+  <si>
+    <t>42/43</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,16 +231,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -269,30 +452,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -342,6 +501,41 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -350,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -371,14 +565,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,7 +592,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG32"/>
+  <dimension ref="A1:AQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,9 +950,15 @@
     <col min="17" max="17" width="10.5703125" customWidth="1"/>
     <col min="18" max="18" width="4.85546875" customWidth="1"/>
     <col min="19" max="19" width="5.7109375" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" customWidth="1"/>
+    <col min="36" max="36" width="8.85546875" customWidth="1"/>
+    <col min="37" max="37" width="9" customWidth="1"/>
+    <col min="41" max="41" width="14.42578125" customWidth="1"/>
+    <col min="42" max="42" width="8.85546875" customWidth="1"/>
+    <col min="43" max="43" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -732,38 +982,38 @@
       <c r="Q1" s="19"/>
       <c r="R1" s="20"/>
       <c r="S1" s="21"/>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AF1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AG1" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="9"/>
@@ -778,7 +1028,7 @@
       <c r="O2" s="9"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="10"/>
-      <c r="S2" s="12"/>
+      <c r="S2" s="9"/>
       <c r="T2" s="6"/>
       <c r="U2" s="7"/>
       <c r="W2" s="6"/>
@@ -790,7 +1040,7 @@
       <c r="AF2" s="6"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="11"/>
       <c r="C3" s="7"/>
@@ -805,7 +1055,7 @@
       <c r="O3" s="7"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="11"/>
-      <c r="S3" s="13"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="6"/>
       <c r="U3" s="7"/>
       <c r="W3" s="6"/>
@@ -816,8 +1066,22 @@
       <c r="AD3" s="7"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="7"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI3" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK3" s="37"/>
+      <c r="AO3" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP3" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ3" s="37"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="11"/>
       <c r="C4" s="7"/>
@@ -832,7 +1096,7 @@
       <c r="O4" s="7"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="13"/>
+      <c r="S4" s="7"/>
       <c r="T4" s="6"/>
       <c r="U4" s="7"/>
       <c r="W4" s="6"/>
@@ -843,8 +1107,26 @@
       <c r="AD4" s="7"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="7"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ4" s="34">
+        <v>37</v>
+      </c>
+      <c r="AK4" s="33">
+        <v>3</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP4" s="39">
+        <v>52</v>
+      </c>
+      <c r="AQ4" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
@@ -859,7 +1141,7 @@
       <c r="O5" s="7"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="13"/>
+      <c r="S5" s="7"/>
       <c r="T5" s="6"/>
       <c r="U5" s="7"/>
       <c r="W5" s="6"/>
@@ -870,8 +1152,26 @@
       <c r="AD5" s="7"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="7"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ5" s="24">
+        <v>36</v>
+      </c>
+      <c r="AK5" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO5" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP5" s="30">
+        <v>51</v>
+      </c>
+      <c r="AQ5" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="11"/>
       <c r="C6" s="7"/>
@@ -886,7 +1186,7 @@
       <c r="O6" s="7"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="11"/>
-      <c r="S6" s="13"/>
+      <c r="S6" s="7"/>
       <c r="T6" s="6"/>
       <c r="U6" s="7"/>
       <c r="W6" s="6"/>
@@ -897,8 +1197,26 @@
       <c r="AD6" s="7"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="7"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ6" s="24">
+        <v>36</v>
+      </c>
+      <c r="AK6" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP6" s="30">
+        <v>51</v>
+      </c>
+      <c r="AQ6" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="11"/>
       <c r="C7" s="7"/>
@@ -913,7 +1231,7 @@
       <c r="O7" s="7"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="11"/>
-      <c r="S7" s="13"/>
+      <c r="S7" s="7"/>
       <c r="T7" s="6"/>
       <c r="U7" s="7"/>
       <c r="W7" s="6"/>
@@ -924,8 +1242,26 @@
       <c r="AD7" s="7"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ7" s="24">
+        <v>35</v>
+      </c>
+      <c r="AK7" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP7" s="30">
+        <v>51</v>
+      </c>
+      <c r="AQ7" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="7"/>
@@ -940,7 +1276,7 @@
       <c r="O8" s="7"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="11"/>
-      <c r="S8" s="13"/>
+      <c r="S8" s="7"/>
       <c r="T8" s="6"/>
       <c r="U8" s="7"/>
       <c r="W8" s="6"/>
@@ -951,8 +1287,26 @@
       <c r="AD8" s="7"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="7"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ8" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK8" s="23">
+        <v>6</v>
+      </c>
+      <c r="AO8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP8" s="30">
+        <v>50</v>
+      </c>
+      <c r="AQ8" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="11"/>
       <c r="C9" s="7"/>
@@ -967,7 +1321,7 @@
       <c r="O9" s="7"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="11"/>
-      <c r="S9" s="13"/>
+      <c r="S9" s="7"/>
       <c r="T9" s="6"/>
       <c r="U9" s="7"/>
       <c r="W9" s="6"/>
@@ -978,8 +1332,26 @@
       <c r="AD9" s="7"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="7"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ9" s="24">
+        <v>33</v>
+      </c>
+      <c r="AK9" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP9" s="30">
+        <v>49</v>
+      </c>
+      <c r="AQ9" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
@@ -994,7 +1366,7 @@
       <c r="O10" s="7"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="11"/>
-      <c r="S10" s="13"/>
+      <c r="S10" s="7"/>
       <c r="T10" s="6"/>
       <c r="U10" s="7"/>
       <c r="W10" s="6"/>
@@ -1005,8 +1377,26 @@
       <c r="AD10" s="7"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="7"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ10" s="24">
+        <v>32</v>
+      </c>
+      <c r="AK10" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO10" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP10" s="30">
+        <v>49</v>
+      </c>
+      <c r="AQ10" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="7"/>
@@ -1021,7 +1411,7 @@
       <c r="O11" s="7"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="11"/>
-      <c r="S11" s="13"/>
+      <c r="S11" s="7"/>
       <c r="T11" s="6"/>
       <c r="U11" s="7"/>
       <c r="W11" s="6"/>
@@ -1032,8 +1422,26 @@
       <c r="AD11" s="7"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="7"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI11" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ11" s="24">
+        <v>31</v>
+      </c>
+      <c r="AK11" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP11" s="30">
+        <v>48</v>
+      </c>
+      <c r="AQ11" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
@@ -1048,7 +1456,7 @@
       <c r="O12" s="7"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="11"/>
-      <c r="S12" s="13"/>
+      <c r="S12" s="7"/>
       <c r="T12" s="6"/>
       <c r="U12" s="7"/>
       <c r="W12" s="6"/>
@@ -1059,8 +1467,26 @@
       <c r="AD12" s="7"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="7"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ12" s="26">
+        <v>30</v>
+      </c>
+      <c r="AK12" s="25">
+        <v>5</v>
+      </c>
+      <c r="AO12" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP12" s="30">
+        <v>48</v>
+      </c>
+      <c r="AQ12" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
@@ -1075,7 +1501,7 @@
       <c r="O13" s="7"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="11"/>
-      <c r="S13" s="13"/>
+      <c r="S13" s="7"/>
       <c r="T13" s="6"/>
       <c r="U13" s="7"/>
       <c r="W13" s="6"/>
@@ -1086,8 +1512,26 @@
       <c r="AD13" s="7"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="7"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ13" s="24">
+        <v>30</v>
+      </c>
+      <c r="AK13" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP13" s="24">
+        <v>47</v>
+      </c>
+      <c r="AQ13" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -1102,7 +1546,7 @@
       <c r="O14" s="7"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="11"/>
-      <c r="S14" s="13"/>
+      <c r="S14" s="7"/>
       <c r="T14" s="6"/>
       <c r="U14" s="7"/>
       <c r="W14" s="6"/>
@@ -1113,8 +1557,26 @@
       <c r="AD14" s="7"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="7"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ14" s="24">
+        <v>29</v>
+      </c>
+      <c r="AK14" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP14" s="24">
+        <v>46</v>
+      </c>
+      <c r="AQ14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -1129,7 +1591,7 @@
       <c r="O15" s="7"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="11"/>
-      <c r="S15" s="13"/>
+      <c r="S15" s="7"/>
       <c r="T15" s="6"/>
       <c r="U15" s="7"/>
       <c r="W15" s="6"/>
@@ -1140,8 +1602,26 @@
       <c r="AD15" s="7"/>
       <c r="AF15" s="6"/>
       <c r="AG15" s="7"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ15" s="24">
+        <v>29</v>
+      </c>
+      <c r="AK15" s="23">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP15" s="24">
+        <v>46</v>
+      </c>
+      <c r="AQ15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -1156,7 +1636,7 @@
       <c r="O16" s="7"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="11"/>
-      <c r="S16" s="13"/>
+      <c r="S16" s="7"/>
       <c r="T16" s="6"/>
       <c r="U16" s="7"/>
       <c r="W16" s="6"/>
@@ -1167,8 +1647,26 @@
       <c r="AD16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="7"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ16" s="24">
+        <v>28</v>
+      </c>
+      <c r="AK16" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP16" s="24">
+        <v>46</v>
+      </c>
+      <c r="AQ16" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -1183,7 +1681,7 @@
       <c r="O17" s="7"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="11"/>
-      <c r="S17" s="13"/>
+      <c r="S17" s="7"/>
       <c r="T17" s="6"/>
       <c r="U17" s="7"/>
       <c r="W17" s="6"/>
@@ -1194,8 +1692,26 @@
       <c r="AD17" s="7"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="7"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ17" s="24">
+        <v>27</v>
+      </c>
+      <c r="AK17" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP17" s="24">
+        <v>45</v>
+      </c>
+      <c r="AQ17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -1210,7 +1726,7 @@
       <c r="O18" s="7"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="11"/>
-      <c r="S18" s="13"/>
+      <c r="S18" s="7"/>
       <c r="T18" s="6"/>
       <c r="U18" s="7"/>
       <c r="W18" s="6"/>
@@ -1221,8 +1737,26 @@
       <c r="AD18" s="7"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="7"/>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ18" s="24">
+        <v>26</v>
+      </c>
+      <c r="AK18" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO18" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP18" s="24">
+        <v>45</v>
+      </c>
+      <c r="AQ18" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
@@ -1237,7 +1771,7 @@
       <c r="O19" s="7"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="11"/>
-      <c r="S19" s="13"/>
+      <c r="S19" s="7"/>
       <c r="T19" s="6"/>
       <c r="U19" s="7"/>
       <c r="W19" s="6"/>
@@ -1248,8 +1782,26 @@
       <c r="AD19" s="7"/>
       <c r="AF19" s="6"/>
       <c r="AG19" s="7"/>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ19" s="24">
+        <v>25</v>
+      </c>
+      <c r="AK19" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO19" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP19" s="24">
+        <v>44</v>
+      </c>
+      <c r="AQ19" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
@@ -1264,7 +1816,7 @@
       <c r="O20" s="7"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="11"/>
-      <c r="S20" s="13"/>
+      <c r="S20" s="7"/>
       <c r="T20" s="6"/>
       <c r="U20" s="7"/>
       <c r="W20" s="6"/>
@@ -1275,8 +1827,26 @@
       <c r="AD20" s="7"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI20" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ20" s="24">
+        <v>24</v>
+      </c>
+      <c r="AK20" s="23">
+        <v>4</v>
+      </c>
+      <c r="AO20" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP20" s="24">
+        <v>44</v>
+      </c>
+      <c r="AQ20" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
@@ -1291,7 +1861,7 @@
       <c r="O21" s="7"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="11"/>
-      <c r="S21" s="13"/>
+      <c r="S21" s="7"/>
       <c r="T21" s="6"/>
       <c r="U21" s="7"/>
       <c r="W21" s="6"/>
@@ -1302,8 +1872,26 @@
       <c r="AD21" s="7"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="7"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ21" s="24">
+        <v>24</v>
+      </c>
+      <c r="AK21" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP21" s="24">
+        <v>43</v>
+      </c>
+      <c r="AQ21" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
@@ -1318,7 +1906,7 @@
       <c r="O22" s="7"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="11"/>
-      <c r="S22" s="13"/>
+      <c r="S22" s="7"/>
       <c r="T22" s="6"/>
       <c r="U22" s="7"/>
       <c r="W22" s="6"/>
@@ -1329,8 +1917,26 @@
       <c r="AD22" s="7"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="7"/>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ22" s="24">
+        <v>23</v>
+      </c>
+      <c r="AK22" s="23">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP22" s="24">
+        <v>43</v>
+      </c>
+      <c r="AQ22" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
@@ -1345,7 +1951,7 @@
       <c r="O23" s="7"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="11"/>
-      <c r="S23" s="13"/>
+      <c r="S23" s="7"/>
       <c r="T23" s="6"/>
       <c r="U23" s="7"/>
       <c r="W23" s="6"/>
@@ -1356,8 +1962,26 @@
       <c r="AD23" s="7"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="7"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ23" s="24">
+        <v>23</v>
+      </c>
+      <c r="AK23" s="23">
+        <v>3</v>
+      </c>
+      <c r="AO23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP23" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ23" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
@@ -1372,7 +1996,7 @@
       <c r="O24" s="7"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="11"/>
-      <c r="S24" s="13"/>
+      <c r="S24" s="7"/>
       <c r="T24" s="6"/>
       <c r="U24" s="7"/>
       <c r="W24" s="6"/>
@@ -1383,8 +2007,26 @@
       <c r="AD24" s="7"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="7"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ24" s="24">
+        <v>18</v>
+      </c>
+      <c r="AK24" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO24" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP24" s="26">
+        <v>42</v>
+      </c>
+      <c r="AQ24" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -1399,7 +2041,7 @@
       <c r="O25" s="7"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="11"/>
-      <c r="S25" s="13"/>
+      <c r="S25" s="7"/>
       <c r="T25" s="6"/>
       <c r="U25" s="7"/>
       <c r="W25" s="6"/>
@@ -1410,8 +2052,26 @@
       <c r="AD25" s="7"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI25" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ25" s="24">
+        <v>18</v>
+      </c>
+      <c r="AK25" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO25" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP25" s="24">
+        <v>42</v>
+      </c>
+      <c r="AQ25" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1426,7 +2086,7 @@
       <c r="O26" s="7"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="11"/>
-      <c r="S26" s="13"/>
+      <c r="S26" s="7"/>
       <c r="T26" s="6"/>
       <c r="U26" s="7"/>
       <c r="W26" s="6"/>
@@ -1437,8 +2097,26 @@
       <c r="AD26" s="7"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="7"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI26" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ26" s="24">
+        <v>17</v>
+      </c>
+      <c r="AK26" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO26" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP26" s="24">
+        <v>41</v>
+      </c>
+      <c r="AQ26" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
@@ -1453,7 +2131,7 @@
       <c r="O27" s="7"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="11"/>
-      <c r="S27" s="13"/>
+      <c r="S27" s="7"/>
       <c r="T27" s="6"/>
       <c r="U27" s="7"/>
       <c r="W27" s="6"/>
@@ -1464,8 +2142,26 @@
       <c r="AD27" s="7"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="7"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI27" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ27" s="24">
+        <v>16</v>
+      </c>
+      <c r="AK27" s="23">
+        <v>2</v>
+      </c>
+      <c r="AO27" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP27" s="24">
+        <v>40</v>
+      </c>
+      <c r="AQ27" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="11"/>
       <c r="C28" s="7"/>
@@ -1480,7 +2176,7 @@
       <c r="O28" s="7"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="11"/>
-      <c r="S28" s="13"/>
+      <c r="S28" s="7"/>
       <c r="T28" s="6"/>
       <c r="U28" s="7"/>
       <c r="W28" s="6"/>
@@ -1491,8 +2187,26 @@
       <c r="AD28" s="7"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="7"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI28" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ28" s="28">
+        <v>16</v>
+      </c>
+      <c r="AK28" s="27">
+        <v>2</v>
+      </c>
+      <c r="AO28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP28" s="24">
+        <v>40</v>
+      </c>
+      <c r="AQ28" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="11"/>
       <c r="C29" s="7"/>
@@ -1507,7 +2221,7 @@
       <c r="O29" s="7"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="11"/>
-      <c r="S29" s="13"/>
+      <c r="S29" s="7"/>
       <c r="T29" s="6"/>
       <c r="U29" s="7"/>
       <c r="W29" s="6"/>
@@ -1518,8 +2232,17 @@
       <c r="AD29" s="7"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="7"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AO29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP29" s="24">
+        <v>39</v>
+      </c>
+      <c r="AQ29" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="7"/>
@@ -1534,7 +2257,7 @@
       <c r="O30" s="7"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="11"/>
-      <c r="S30" s="13"/>
+      <c r="S30" s="7"/>
       <c r="T30" s="6"/>
       <c r="U30" s="7"/>
       <c r="W30" s="6"/>
@@ -1545,8 +2268,17 @@
       <c r="AD30" s="7"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="7"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AO30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP30" s="24">
+        <v>39</v>
+      </c>
+      <c r="AQ30" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7"/>
@@ -1561,7 +2293,7 @@
       <c r="O31" s="7"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="11"/>
-      <c r="S31" s="13"/>
+      <c r="S31" s="7"/>
       <c r="T31" s="6"/>
       <c r="U31" s="7"/>
       <c r="W31" s="6"/>
@@ -1573,7 +2305,7 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="7"/>
     </row>
-    <row r="32" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7"/>
@@ -1586,19 +2318,19 @@
       <c r="M32" s="6"/>
       <c r="N32" s="11"/>
       <c r="O32" s="7"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="23"/>
-      <c r="W32" s="22"/>
-      <c r="X32" s="23"/>
-      <c r="Z32" s="22"/>
-      <c r="AA32" s="23"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="23"/>
-      <c r="AF32" s="22"/>
-      <c r="AG32" s="23"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="15"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="15"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="15"/>
+      <c r="AC32" s="14"/>
+      <c r="AD32" s="15"/>
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
more mods to plan
</commit_message>
<xml_diff>
--- a/Tools/Clerk Blank.xlsx
+++ b/Tools/Clerk Blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E7ABFA-CC3F-4BD3-ACA9-C2C182CA1C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3903D1-95B5-444E-904F-58DB8688C6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -573,24 +573,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,12 +598,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,6 +618,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS19" sqref="AS19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,29 +953,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="E1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-      <c r="I1" s="16" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="M1" s="16" t="s">
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
+      <c r="M1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="21"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="34"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="37"/>
       <c r="T1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1066,20 +1060,20 @@
       <c r="AD3" s="7"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="7"/>
-      <c r="AI3" s="35" t="s">
+      <c r="AI3" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="AJ3" s="36" t="s">
+      <c r="AJ3" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="AK3" s="37"/>
-      <c r="AO3" s="35" t="s">
+      <c r="AK3" s="29"/>
+      <c r="AO3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AP3" s="36" t="s">
+      <c r="AP3" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="AQ3" s="37"/>
+      <c r="AQ3" s="29"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1107,22 +1101,22 @@
       <c r="AD4" s="7"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="7"/>
-      <c r="AI4" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ4" s="34">
-        <v>37</v>
-      </c>
-      <c r="AK4" s="33">
-        <v>3</v>
-      </c>
-      <c r="AO4" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP4" s="39">
-        <v>52</v>
-      </c>
-      <c r="AQ4" s="38">
+      <c r="AI4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="22">
+        <v>16</v>
+      </c>
+      <c r="AK4" s="21">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP4" s="18">
+        <v>39</v>
+      </c>
+      <c r="AQ4" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1152,23 +1146,23 @@
       <c r="AD5" s="7"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="7"/>
-      <c r="AI5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ5" s="24">
-        <v>36</v>
-      </c>
-      <c r="AK5" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO5" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP5" s="30">
-        <v>51</v>
-      </c>
-      <c r="AQ5" s="29">
+      <c r="AI5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ5" s="18">
+        <v>16</v>
+      </c>
+      <c r="AK5" s="17">
         <v>2</v>
+      </c>
+      <c r="AO5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP5" s="18">
+        <v>39</v>
+      </c>
+      <c r="AQ5" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
@@ -1197,23 +1191,23 @@
       <c r="AD6" s="7"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="7"/>
-      <c r="AI6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ6" s="24">
-        <v>36</v>
-      </c>
-      <c r="AK6" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO6" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP6" s="30">
-        <v>51</v>
-      </c>
-      <c r="AQ6" s="29">
-        <v>1</v>
+      <c r="AI6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ6" s="18">
+        <v>17</v>
+      </c>
+      <c r="AK6" s="17">
+        <v>2</v>
+      </c>
+      <c r="AO6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP6" s="18">
+        <v>40</v>
+      </c>
+      <c r="AQ6" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
@@ -1242,23 +1236,23 @@
       <c r="AD7" s="7"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
-      <c r="AI7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ7" s="24">
-        <v>35</v>
-      </c>
-      <c r="AK7" s="23">
+      <c r="AI7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ7" s="18">
+        <v>18</v>
+      </c>
+      <c r="AK7" s="17">
         <v>2</v>
       </c>
-      <c r="AO7" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP7" s="30">
-        <v>51</v>
-      </c>
-      <c r="AQ7" s="29">
-        <v>1</v>
+      <c r="AO7" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP7" s="18">
+        <v>40</v>
+      </c>
+      <c r="AQ7" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
@@ -1287,23 +1281,23 @@
       <c r="AD8" s="7"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="7"/>
-      <c r="AI8" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ8" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK8" s="23">
-        <v>6</v>
-      </c>
-      <c r="AO8" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP8" s="30">
-        <v>50</v>
-      </c>
-      <c r="AQ8" s="29">
-        <v>3</v>
+      <c r="AI8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ8" s="18">
+        <v>18</v>
+      </c>
+      <c r="AK8" s="17">
+        <v>2</v>
+      </c>
+      <c r="AO8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP8" s="18">
+        <v>41</v>
+      </c>
+      <c r="AQ8" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
@@ -1332,23 +1326,23 @@
       <c r="AD9" s="7"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="7"/>
-      <c r="AI9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ9" s="24">
-        <v>33</v>
-      </c>
-      <c r="AK9" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO9" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP9" s="30">
-        <v>49</v>
-      </c>
-      <c r="AQ9" s="29">
-        <v>2</v>
+      <c r="AI9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ9" s="18">
+        <v>23</v>
+      </c>
+      <c r="AK9" s="17">
+        <v>3</v>
+      </c>
+      <c r="AO9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP9" s="18">
+        <v>42</v>
+      </c>
+      <c r="AQ9" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1377,22 +1371,22 @@
       <c r="AD10" s="7"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="7"/>
-      <c r="AI10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ10" s="24">
-        <v>32</v>
-      </c>
-      <c r="AK10" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO10" s="32" t="s">
+      <c r="AI10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ10" s="18">
+        <v>23</v>
+      </c>
+      <c r="AK10" s="17">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AP10" s="30">
-        <v>49</v>
-      </c>
-      <c r="AQ10" s="29">
+      <c r="AP10" s="20">
+        <v>42</v>
+      </c>
+      <c r="AQ10" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1422,22 +1416,22 @@
       <c r="AD11" s="7"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="7"/>
-      <c r="AI11" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ11" s="24">
-        <v>31</v>
-      </c>
-      <c r="AK11" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO11" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP11" s="30">
-        <v>48</v>
-      </c>
-      <c r="AQ11" s="29">
+      <c r="AI11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ11" s="18">
+        <v>24</v>
+      </c>
+      <c r="AK11" s="17">
+        <v>2</v>
+      </c>
+      <c r="AO11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ11" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1467,22 +1461,22 @@
       <c r="AD12" s="7"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="7"/>
-      <c r="AI12" s="25" t="s">
+      <c r="AI12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ12" s="18">
+        <v>24</v>
+      </c>
+      <c r="AK12" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AJ12" s="26">
-        <v>30</v>
-      </c>
-      <c r="AK12" s="25">
-        <v>5</v>
-      </c>
-      <c r="AO12" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP12" s="30">
-        <v>48</v>
-      </c>
-      <c r="AQ12" s="29">
+      <c r="AP12" s="18">
+        <v>43</v>
+      </c>
+      <c r="AQ12" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1512,23 +1506,23 @@
       <c r="AD13" s="7"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="7"/>
-      <c r="AI13" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ13" s="24">
-        <v>30</v>
-      </c>
-      <c r="AK13" s="23">
+      <c r="AI13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ13" s="18">
+        <v>25</v>
+      </c>
+      <c r="AK13" s="17">
         <v>4</v>
       </c>
-      <c r="AO13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP13" s="24">
-        <v>47</v>
-      </c>
-      <c r="AQ13" s="23">
-        <v>2</v>
+      <c r="AO13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP13" s="18">
+        <v>43</v>
+      </c>
+      <c r="AQ13" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
@@ -1557,23 +1551,23 @@
       <c r="AD14" s="7"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="7"/>
-      <c r="AI14" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ14" s="24">
-        <v>29</v>
-      </c>
-      <c r="AK14" s="23">
+      <c r="AI14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ14" s="18">
+        <v>26</v>
+      </c>
+      <c r="AK14" s="17">
         <v>4</v>
       </c>
-      <c r="AO14" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP14" s="24">
-        <v>46</v>
-      </c>
-      <c r="AQ14" s="23">
-        <v>1</v>
+      <c r="AO14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP14" s="18">
+        <v>44</v>
+      </c>
+      <c r="AQ14" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
@@ -1602,22 +1596,22 @@
       <c r="AD15" s="7"/>
       <c r="AF15" s="6"/>
       <c r="AG15" s="7"/>
-      <c r="AI15" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ15" s="24">
-        <v>29</v>
-      </c>
-      <c r="AK15" s="23">
-        <v>1</v>
-      </c>
-      <c r="AO15" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP15" s="24">
+      <c r="AI15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ15" s="18">
+        <v>27</v>
+      </c>
+      <c r="AK15" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="AQ15" s="23">
+      <c r="AP15" s="18">
+        <v>44</v>
+      </c>
+      <c r="AQ15" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1647,23 +1641,23 @@
       <c r="AD16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="7"/>
-      <c r="AI16" s="23" t="s">
+      <c r="AI16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AJ16" s="24">
+      <c r="AJ16" s="18">
         <v>28</v>
       </c>
-      <c r="AK16" s="23">
+      <c r="AK16" s="17">
         <v>4</v>
       </c>
-      <c r="AO16" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP16" s="24">
-        <v>46</v>
-      </c>
-      <c r="AQ16" s="23">
-        <v>1</v>
+      <c r="AO16" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP16" s="18">
+        <v>45</v>
+      </c>
+      <c r="AQ16" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
@@ -1692,22 +1686,22 @@
       <c r="AD17" s="7"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="7"/>
-      <c r="AI17" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ17" s="24">
-        <v>27</v>
-      </c>
-      <c r="AK17" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO17" s="23" t="s">
+      <c r="AI17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AP17" s="24">
+      <c r="AJ17" s="18">
+        <v>29</v>
+      </c>
+      <c r="AK17" s="17">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP17" s="18">
         <v>45</v>
       </c>
-      <c r="AQ17" s="23">
+      <c r="AQ17" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1737,23 +1731,23 @@
       <c r="AD18" s="7"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="7"/>
-      <c r="AI18" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ18" s="24">
-        <v>26</v>
-      </c>
-      <c r="AK18" s="23">
+      <c r="AI18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ18" s="18">
+        <v>29</v>
+      </c>
+      <c r="AK18" s="17">
         <v>4</v>
       </c>
-      <c r="AO18" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP18" s="24">
-        <v>45</v>
-      </c>
-      <c r="AQ18" s="23">
-        <v>2</v>
+      <c r="AO18" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP18" s="18">
+        <v>46</v>
+      </c>
+      <c r="AQ18" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
@@ -1782,22 +1776,22 @@
       <c r="AD19" s="7"/>
       <c r="AF19" s="6"/>
       <c r="AG19" s="7"/>
-      <c r="AI19" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ19" s="24">
-        <v>25</v>
-      </c>
-      <c r="AK19" s="23">
+      <c r="AI19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ19" s="18">
+        <v>30</v>
+      </c>
+      <c r="AK19" s="17">
         <v>4</v>
       </c>
-      <c r="AO19" s="23" t="s">
+      <c r="AO19" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP19" s="18">
         <v>46</v>
       </c>
-      <c r="AP19" s="24">
-        <v>44</v>
-      </c>
-      <c r="AQ19" s="23">
+      <c r="AQ19" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1827,23 +1821,23 @@
       <c r="AD20" s="7"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
-      <c r="AI20" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ20" s="24">
-        <v>24</v>
-      </c>
-      <c r="AK20" s="23">
-        <v>4</v>
-      </c>
-      <c r="AO20" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="AP20" s="24">
-        <v>44</v>
-      </c>
-      <c r="AQ20" s="23">
-        <v>2</v>
+      <c r="AI20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ20" s="20">
+        <v>30</v>
+      </c>
+      <c r="AK20" s="19">
+        <v>5</v>
+      </c>
+      <c r="AO20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP20" s="18">
+        <v>46</v>
+      </c>
+      <c r="AQ20" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
@@ -1872,23 +1866,23 @@
       <c r="AD21" s="7"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="7"/>
-      <c r="AI21" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ21" s="24">
-        <v>24</v>
-      </c>
-      <c r="AK21" s="23">
+      <c r="AI21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ21" s="18">
+        <v>31</v>
+      </c>
+      <c r="AK21" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO21" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP21" s="18">
+        <v>47</v>
+      </c>
+      <c r="AQ21" s="17">
         <v>2</v>
-      </c>
-      <c r="AO21" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP21" s="24">
-        <v>43</v>
-      </c>
-      <c r="AQ21" s="23">
-        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
@@ -1917,20 +1911,20 @@
       <c r="AD22" s="7"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="7"/>
-      <c r="AI22" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ22" s="24">
-        <v>23</v>
-      </c>
-      <c r="AK22" s="23">
-        <v>1</v>
+      <c r="AI22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ22" s="18">
+        <v>32</v>
+      </c>
+      <c r="AK22" s="17">
+        <v>4</v>
       </c>
       <c r="AO22" s="23" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AP22" s="24">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="AQ22" s="23">
         <v>1</v>
@@ -1962,20 +1956,20 @@
       <c r="AD23" s="7"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="7"/>
-      <c r="AI23" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ23" s="24">
-        <v>23</v>
-      </c>
-      <c r="AK23" s="23">
-        <v>3</v>
+      <c r="AI23" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ23" s="18">
+        <v>33</v>
+      </c>
+      <c r="AK23" s="17">
+        <v>4</v>
       </c>
       <c r="AO23" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP23" s="24" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="AP23" s="24">
+        <v>48</v>
       </c>
       <c r="AQ23" s="23">
         <v>2</v>
@@ -2007,22 +2001,22 @@
       <c r="AD24" s="7"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="7"/>
-      <c r="AI24" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ24" s="24">
-        <v>18</v>
-      </c>
-      <c r="AK24" s="23">
-        <v>2</v>
-      </c>
-      <c r="AO24" s="25" t="s">
+      <c r="AI24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ24" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK24" s="17">
+        <v>6</v>
+      </c>
+      <c r="AO24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AP24" s="26">
-        <v>42</v>
-      </c>
-      <c r="AQ24" s="25">
+      <c r="AP24" s="24">
+        <v>49</v>
+      </c>
+      <c r="AQ24" s="23">
         <v>1</v>
       </c>
     </row>
@@ -2052,23 +2046,23 @@
       <c r="AD25" s="7"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
-      <c r="AI25" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ25" s="24">
-        <v>18</v>
-      </c>
-      <c r="AK25" s="23">
+      <c r="AI25" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ25" s="18">
+        <v>35</v>
+      </c>
+      <c r="AK25" s="17">
         <v>2</v>
       </c>
       <c r="AO25" s="23" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="AP25" s="24">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AQ25" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
@@ -2097,23 +2091,23 @@
       <c r="AD26" s="7"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="7"/>
-      <c r="AI26" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ26" s="24">
-        <v>17</v>
-      </c>
-      <c r="AK26" s="23">
-        <v>2</v>
+      <c r="AI26" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ26" s="18">
+        <v>36</v>
+      </c>
+      <c r="AK26" s="17">
+        <v>4</v>
       </c>
       <c r="AO26" s="23" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="AP26" s="24">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AQ26" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -2142,23 +2136,23 @@
       <c r="AD27" s="7"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="7"/>
-      <c r="AI27" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ27" s="24">
-        <v>16</v>
-      </c>
-      <c r="AK27" s="23">
-        <v>2</v>
+      <c r="AI27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ27" s="18">
+        <v>36</v>
+      </c>
+      <c r="AK27" s="17">
+        <v>4</v>
       </c>
       <c r="AO27" s="23" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="AP27" s="24">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AQ27" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
@@ -2187,23 +2181,23 @@
       <c r="AD28" s="7"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="7"/>
-      <c r="AI28" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ28" s="28">
-        <v>16</v>
-      </c>
-      <c r="AK28" s="27">
-        <v>2</v>
+      <c r="AI28" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ28" s="26">
+        <v>37</v>
+      </c>
+      <c r="AK28" s="25">
+        <v>3</v>
       </c>
       <c r="AO28" s="23" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="AP28" s="24">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AQ28" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
@@ -2233,13 +2227,13 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="7"/>
       <c r="AO29" s="23" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="AP29" s="24">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="AQ29" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
@@ -2268,13 +2262,13 @@
       <c r="AD30" s="7"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="7"/>
-      <c r="AO30" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP30" s="24">
-        <v>39</v>
-      </c>
-      <c r="AQ30" s="23">
+      <c r="AO30" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP30" s="31">
+        <v>52</v>
+      </c>
+      <c r="AQ30" s="30">
         <v>2</v>
       </c>
     </row>
@@ -2319,7 +2313,7 @@
       <c r="N32" s="11"/>
       <c r="O32" s="7"/>
       <c r="Q32" s="14"/>
-      <c r="R32" s="22"/>
+      <c r="R32" s="16"/>
       <c r="S32" s="15"/>
       <c r="T32" s="14"/>
       <c r="U32" s="15"/>

</xml_diff>

<commit_message>
Clerk Blank updated new stages
</commit_message>
<xml_diff>
--- a/Tools/Clerk Blank.xlsx
+++ b/Tools/Clerk Blank.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links-1\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CE44A9-BE57-43BE-8655-7EFA031F17BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114FC856-F865-4F70-8511-5924DB46DF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12645" yWindow="3870" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Staged Loaded Average</t>
   </si>
@@ -58,36 +67,15 @@
     <t>PAGER</t>
   </si>
   <si>
-    <t>RM-HV</t>
-  </si>
-  <si>
-    <t>DBS3-MR</t>
-  </si>
-  <si>
-    <t>DBS2-MR</t>
-  </si>
-  <si>
-    <t>DBI4-ND</t>
-  </si>
-  <si>
     <t>STN8</t>
   </si>
   <si>
-    <t>JP Carts</t>
-  </si>
-  <si>
     <t>DSN1-ND</t>
   </si>
   <si>
     <t>BHX8</t>
   </si>
   <si>
-    <t>DBI5-MR</t>
-  </si>
-  <si>
-    <t>DWR1-MR</t>
-  </si>
-  <si>
     <t>DEX2-ND</t>
   </si>
   <si>
@@ -103,30 +91,6 @@
     <t>UPS</t>
   </si>
   <si>
-    <t>DPD</t>
-  </si>
-  <si>
-    <t>BFSA</t>
-  </si>
-  <si>
-    <t>RM-H1</t>
-  </si>
-  <si>
-    <t>BRISTOL2</t>
-  </si>
-  <si>
-    <t>CARDIFF</t>
-  </si>
-  <si>
-    <t>EXETER</t>
-  </si>
-  <si>
-    <t>PLYMOUTH</t>
-  </si>
-  <si>
-    <t>SWANSEA</t>
-  </si>
-  <si>
     <t>DRH1-ND</t>
   </si>
   <si>
@@ -151,15 +115,9 @@
     <t>DNN1-ND</t>
   </si>
   <si>
-    <t>DBI2-ND</t>
-  </si>
-  <si>
     <t>DPO1-ND</t>
   </si>
   <si>
-    <t>DCR2-ND</t>
-  </si>
-  <si>
     <t>DSO2-ND</t>
   </si>
   <si>
@@ -175,30 +133,12 @@
     <t>DCF1-ND</t>
   </si>
   <si>
-    <t>DRG2-ND</t>
-  </si>
-  <si>
-    <t>DHA1-ND</t>
-  </si>
-  <si>
     <t>SEH1</t>
   </si>
   <si>
-    <t>DXM2-ND</t>
-  </si>
-  <si>
     <t>DEX2-SD</t>
   </si>
   <si>
-    <t>DBI7-ND</t>
-  </si>
-  <si>
-    <t>34/35</t>
-  </si>
-  <si>
-    <t>42/43</t>
-  </si>
-  <si>
     <t>Lane</t>
   </si>
   <si>
@@ -206,13 +146,94 @@
   </si>
   <si>
     <t xml:space="preserve">Lane </t>
+  </si>
+  <si>
+    <t>RM-TRURO-GB-H2</t>
+  </si>
+  <si>
+    <t>RM-SWANSEA-GB-H2</t>
+  </si>
+  <si>
+    <t>RM-PLYMOUTH-GB-H2</t>
+  </si>
+  <si>
+    <t>15/16</t>
+  </si>
+  <si>
+    <t>RM-EXETER-GB-H2</t>
+  </si>
+  <si>
+    <t>16/17</t>
+  </si>
+  <si>
+    <t>RM-CARDIFF-GB-H2</t>
+  </si>
+  <si>
+    <t>17/18</t>
+  </si>
+  <si>
+    <t>RM-BRISTOL2-GB-H2</t>
+  </si>
+  <si>
+    <t>RM-BRISTOL-GB-H1</t>
+  </si>
+  <si>
+    <t>AIR-BRS2-EMSA</t>
+  </si>
+  <si>
+    <t>DPD-BURBAGE-GB-H1</t>
+  </si>
+  <si>
+    <t>DXN1-ND</t>
+  </si>
+  <si>
+    <t>DWR1-DCE1-ND-MR</t>
+  </si>
+  <si>
+    <t>DHA1-DCR2-ND-MR</t>
+  </si>
+  <si>
+    <t>DBS3-ND</t>
+  </si>
+  <si>
+    <t>DBS2-ND</t>
+  </si>
+  <si>
+    <t>DST1-ND</t>
+  </si>
+  <si>
+    <t>LMC</t>
+  </si>
+  <si>
+    <t>DXE1-ND</t>
+  </si>
+  <si>
+    <t>DBI2-DBI7-MR-ND</t>
+  </si>
+  <si>
+    <t>DXM2-DPR1-MR-ND</t>
+  </si>
+  <si>
+    <t>DOX2-ND</t>
+  </si>
+  <si>
+    <t>DRG2-DXW2-MR-ND</t>
+  </si>
+  <si>
+    <t>DBI5-ND</t>
+  </si>
+  <si>
+    <t>DIG1-ND</t>
+  </si>
+  <si>
+    <t>DPE2-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,11 +256,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -253,15 +269,11 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -278,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -524,35 +536,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -585,46 +573,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,10 +597,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -934,7 +895,7 @@
   <dimension ref="A1:AQ32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO32" sqref="AO32"/>
+      <selection activeCell="BB29" sqref="BB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,38 +919,39 @@
     <col min="17" max="17" width="10.5703125" customWidth="1"/>
     <col min="18" max="18" width="4.85546875" customWidth="1"/>
     <col min="19" max="19" width="5.7109375" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" customWidth="1"/>
+    <col min="35" max="35" width="20.42578125" customWidth="1"/>
     <col min="36" max="36" width="8.85546875" customWidth="1"/>
-    <col min="37" max="37" width="9" customWidth="1"/>
-    <col min="41" max="41" width="14.42578125" customWidth="1"/>
+    <col min="37" max="37" width="7.140625" customWidth="1"/>
+    <col min="40" max="40" width="6.28515625" customWidth="1"/>
+    <col min="41" max="41" width="19.28515625" customWidth="1"/>
     <col min="42" max="42" width="8.85546875" customWidth="1"/>
     <col min="43" max="43" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-      <c r="E1" s="32" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="E1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="I1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
-      <c r="M1" s="32" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
+      <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="37"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="25"/>
       <c r="T1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1021,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="10"/>
       <c r="C2" s="9"/>
@@ -1048,7 +1010,7 @@
       <c r="AF2" s="6"/>
       <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="11"/>
       <c r="C3" s="7"/>
@@ -1074,20 +1036,20 @@
       <c r="AD3" s="7"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="7"/>
-      <c r="AI3" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ3" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK3" s="29"/>
-      <c r="AO3" s="27" t="s">
-        <v>59</v>
+      <c r="AI3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK3" s="30"/>
+      <c r="AO3" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="AP3" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ3" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="AQ3" s="28"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1115,19 +1077,19 @@
       <c r="AD4" s="7"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="7"/>
-      <c r="AI4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ4" s="22">
-        <v>16</v>
-      </c>
-      <c r="AK4" s="21">
+      <c r="AI4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ4" s="29">
+        <v>14</v>
+      </c>
+      <c r="AK4" s="18">
         <v>2</v>
       </c>
-      <c r="AO4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP4" s="18">
+      <c r="AO4" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP4" s="29">
         <v>39</v>
       </c>
       <c r="AQ4" s="17">
@@ -1160,19 +1122,19 @@
       <c r="AD5" s="7"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="7"/>
-      <c r="AI5" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ5" s="18">
-        <v>16</v>
+      <c r="AI5" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ5" s="29">
+        <v>15</v>
       </c>
       <c r="AK5" s="17">
         <v>2</v>
       </c>
-      <c r="AO5" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP5" s="18">
+      <c r="AO5" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP5" s="29">
         <v>39</v>
       </c>
       <c r="AQ5" s="17">
@@ -1205,19 +1167,19 @@
       <c r="AD6" s="7"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="7"/>
-      <c r="AI6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ6" s="18">
-        <v>17</v>
+      <c r="AI6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="AK6" s="17">
         <v>2</v>
       </c>
-      <c r="AO6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP6" s="18">
+      <c r="AO6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP6" s="29">
         <v>40</v>
       </c>
       <c r="AQ6" s="17">
@@ -1250,20 +1212,20 @@
       <c r="AD7" s="7"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
-      <c r="AI7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ7" s="18">
-        <v>18</v>
+      <c r="AI7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ7" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="AK7" s="17">
         <v>2</v>
       </c>
-      <c r="AO7" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP7" s="18">
-        <v>40</v>
+      <c r="AO7" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP7" s="29">
+        <v>41</v>
       </c>
       <c r="AQ7" s="17">
         <v>2</v>
@@ -1295,19 +1257,19 @@
       <c r="AD8" s="7"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="7"/>
-      <c r="AI8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ8" s="18">
-        <v>18</v>
+      <c r="AI8" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ8" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="AK8" s="17">
         <v>2</v>
       </c>
-      <c r="AO8" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP8" s="18">
+      <c r="AO8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP8" s="29">
         <v>41</v>
       </c>
       <c r="AQ8" s="17">
@@ -1340,19 +1302,19 @@
       <c r="AD9" s="7"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="7"/>
-      <c r="AI9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ9" s="18">
-        <v>23</v>
+      <c r="AI9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ9" s="29">
+        <v>18</v>
       </c>
       <c r="AK9" s="17">
         <v>3</v>
       </c>
-      <c r="AO9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP9" s="18">
+      <c r="AO9" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP9" s="29">
         <v>42</v>
       </c>
       <c r="AQ9" s="17">
@@ -1385,22 +1347,22 @@
       <c r="AD10" s="7"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="7"/>
-      <c r="AI10" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ10" s="18">
+      <c r="AI10" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ10" s="29">
         <v>23</v>
       </c>
       <c r="AK10" s="17">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP10" s="20">
+        <v>2</v>
+      </c>
+      <c r="AO10" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP10" s="29">
         <v>42</v>
       </c>
-      <c r="AQ10" s="19">
+      <c r="AQ10" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1430,20 +1392,20 @@
       <c r="AD11" s="7"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="7"/>
-      <c r="AI11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ11" s="18">
-        <v>24</v>
+      <c r="AI11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ11" s="29">
+        <v>23</v>
       </c>
       <c r="AK11" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO11" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP11" s="18" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="AO11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP11" s="29">
+        <v>43</v>
       </c>
       <c r="AQ11" s="17">
         <v>2</v>
@@ -1475,19 +1437,19 @@
       <c r="AD12" s="7"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="7"/>
-      <c r="AI12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ12" s="18">
+      <c r="AI12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ12" s="29">
         <v>24</v>
       </c>
       <c r="AK12" s="17">
         <v>4</v>
       </c>
-      <c r="AO12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP12" s="18">
+      <c r="AO12" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP12" s="29">
         <v>43</v>
       </c>
       <c r="AQ12" s="17">
@@ -1520,20 +1482,20 @@
       <c r="AD13" s="7"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="7"/>
-      <c r="AI13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ13" s="18">
-        <v>25</v>
+      <c r="AI13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ13" s="29">
+        <v>24</v>
       </c>
       <c r="AK13" s="17">
         <v>4</v>
       </c>
-      <c r="AO13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="AP13" s="18">
-        <v>43</v>
+      <c r="AO13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP13" s="29">
+        <v>44</v>
       </c>
       <c r="AQ13" s="17">
         <v>1</v>
@@ -1565,19 +1527,19 @@
       <c r="AD14" s="7"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="7"/>
-      <c r="AI14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ14" s="18">
-        <v>26</v>
+      <c r="AI14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ14" s="29">
+        <v>25</v>
       </c>
       <c r="AK14" s="17">
         <v>4</v>
       </c>
-      <c r="AO14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP14" s="18">
+      <c r="AO14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP14" s="29">
         <v>44</v>
       </c>
       <c r="AQ14" s="17">
@@ -1610,20 +1572,20 @@
       <c r="AD15" s="7"/>
       <c r="AF15" s="6"/>
       <c r="AG15" s="7"/>
-      <c r="AI15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ15" s="18">
-        <v>27</v>
+      <c r="AI15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ15" s="29">
+        <v>26</v>
       </c>
       <c r="AK15" s="17">
         <v>4</v>
       </c>
-      <c r="AO15" s="17" t="s">
+      <c r="AO15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP15" s="29">
         <v>45</v>
-      </c>
-      <c r="AP15" s="18">
-        <v>44</v>
       </c>
       <c r="AQ15" s="17">
         <v>1</v>
@@ -1655,19 +1617,19 @@
       <c r="AD16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="7"/>
-      <c r="AI16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ16" s="18">
-        <v>28</v>
+      <c r="AI16" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ16" s="29">
+        <v>27</v>
       </c>
       <c r="AK16" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO16" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP16" s="18">
+        <v>2</v>
+      </c>
+      <c r="AO16" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP16" s="29">
         <v>45</v>
       </c>
       <c r="AQ16" s="17">
@@ -1700,20 +1662,20 @@
       <c r="AD17" s="7"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="7"/>
-      <c r="AI17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ17" s="18">
-        <v>29</v>
+      <c r="AI17" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ17" s="29">
+        <v>28</v>
       </c>
       <c r="AK17" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP17" s="18">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="AO17" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP17" s="29">
+        <v>46</v>
       </c>
       <c r="AQ17" s="17">
         <v>1</v>
@@ -1745,19 +1707,19 @@
       <c r="AD18" s="7"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="7"/>
-      <c r="AI18" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ18" s="18">
+      <c r="AI18" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ18" s="29">
         <v>29</v>
       </c>
       <c r="AK18" s="17">
         <v>4</v>
       </c>
-      <c r="AO18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP18" s="18">
+      <c r="AO18" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP18" s="29">
         <v>46</v>
       </c>
       <c r="AQ18" s="17">
@@ -1790,20 +1752,20 @@
       <c r="AD19" s="7"/>
       <c r="AF19" s="6"/>
       <c r="AG19" s="7"/>
-      <c r="AI19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ19" s="18">
+      <c r="AI19" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ19" s="29">
         <v>30</v>
       </c>
       <c r="AK19" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO19" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP19" s="18">
-        <v>46</v>
+        <v>5</v>
+      </c>
+      <c r="AO19" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP19" s="29">
+        <v>47</v>
       </c>
       <c r="AQ19" s="17">
         <v>1</v>
@@ -1835,20 +1797,20 @@
       <c r="AD20" s="7"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
-      <c r="AI20" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ20" s="20">
-        <v>30</v>
-      </c>
-      <c r="AK20" s="19">
-        <v>5</v>
-      </c>
-      <c r="AO20" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP20" s="18">
-        <v>46</v>
+      <c r="AI20" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ20" s="29">
+        <v>31</v>
+      </c>
+      <c r="AK20" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO20" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP20" s="29">
+        <v>47</v>
       </c>
       <c r="AQ20" s="17">
         <v>1</v>
@@ -1880,23 +1842,23 @@
       <c r="AD21" s="7"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="7"/>
-      <c r="AI21" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ21" s="18">
-        <v>31</v>
+      <c r="AI21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ21" s="29">
+        <v>32</v>
       </c>
       <c r="AK21" s="17">
         <v>4</v>
       </c>
-      <c r="AO21" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP21" s="18">
-        <v>47</v>
+      <c r="AO21" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP21" s="29">
+        <v>48</v>
       </c>
       <c r="AQ21" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
@@ -1925,20 +1887,22 @@
       <c r="AD22" s="7"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="7"/>
-      <c r="AI22" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ22" s="18">
-        <v>32</v>
+      <c r="AI22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ22" s="29">
+        <v>33</v>
       </c>
       <c r="AK22" s="17">
         <v>4</v>
       </c>
-      <c r="AO22" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP22" s="39"/>
-      <c r="AQ22" s="38">
+      <c r="AO22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP22" s="29">
+        <v>49</v>
+      </c>
+      <c r="AQ22" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1968,23 +1932,23 @@
       <c r="AD23" s="7"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="7"/>
-      <c r="AI23" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ23" s="18">
-        <v>33</v>
+      <c r="AI23" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ23" s="29">
+        <v>34</v>
       </c>
       <c r="AK23" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO23" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP23" s="24">
-        <v>48</v>
-      </c>
-      <c r="AQ23" s="23">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="AO23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP23" s="29">
+        <v>50</v>
+      </c>
+      <c r="AQ23" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
@@ -2013,23 +1977,23 @@
       <c r="AD24" s="7"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="7"/>
-      <c r="AI24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ24" s="18" t="s">
-        <v>55</v>
+      <c r="AI24" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ24" s="29">
+        <v>35</v>
       </c>
       <c r="AK24" s="17">
-        <v>6</v>
-      </c>
-      <c r="AO24" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP24" s="24">
-        <v>49</v>
-      </c>
-      <c r="AQ24" s="23">
         <v>2</v>
+      </c>
+      <c r="AO24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP24" s="29">
+        <v>50</v>
+      </c>
+      <c r="AQ24" s="19">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
@@ -2058,23 +2022,23 @@
       <c r="AD25" s="7"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
-      <c r="AI25" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ25" s="18">
-        <v>35</v>
+      <c r="AI25" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ25" s="29">
+        <v>36</v>
       </c>
       <c r="AK25" s="17">
         <v>2</v>
       </c>
-      <c r="AO25" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP25" s="24">
-        <v>50</v>
-      </c>
-      <c r="AQ25" s="23">
-        <v>3</v>
+      <c r="AO25" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP25" s="29">
+        <v>51</v>
+      </c>
+      <c r="AQ25" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
@@ -2103,22 +2067,22 @@
       <c r="AD26" s="7"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="7"/>
-      <c r="AI26" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ26" s="18">
-        <v>36</v>
+      <c r="AI26" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ26" s="29">
+        <v>37</v>
       </c>
       <c r="AK26" s="17">
         <v>2</v>
       </c>
-      <c r="AO26" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP26" s="24">
+      <c r="AO26" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP26" s="29">
         <v>51</v>
       </c>
-      <c r="AQ26" s="23">
+      <c r="AQ26" s="19">
         <v>1</v>
       </c>
     </row>
@@ -2148,23 +2112,23 @@
       <c r="AD27" s="7"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="7"/>
-      <c r="AI27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ27" s="18">
-        <v>36</v>
+      <c r="AI27" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ27" s="29">
+        <v>37</v>
       </c>
       <c r="AK27" s="17">
+        <v>3</v>
+      </c>
+      <c r="AO27" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP27" s="29">
+        <v>52</v>
+      </c>
+      <c r="AQ27" s="19">
         <v>2</v>
-      </c>
-      <c r="AO27" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP27" s="24">
-        <v>51</v>
-      </c>
-      <c r="AQ27" s="23">
-        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
@@ -2193,24 +2157,6 @@
       <c r="AD28" s="7"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="7"/>
-      <c r="AI28" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ28" s="26">
-        <v>37</v>
-      </c>
-      <c r="AK28" s="25">
-        <v>3</v>
-      </c>
-      <c r="AO28" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP28" s="24">
-        <v>51</v>
-      </c>
-      <c r="AQ28" s="23">
-        <v>2</v>
-      </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
@@ -2238,15 +2184,9 @@
       <c r="AD29" s="7"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="7"/>
-      <c r="AO29" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP29" s="31">
-        <v>52</v>
-      </c>
-      <c r="AQ29" s="30">
-        <v>2</v>
-      </c>
+      <c r="AO29" s="26"/>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="26"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>

</xml_diff>

<commit_message>
Updated Staging area and optimal bays
</commit_message>
<xml_diff>
--- a/Tools/Clerk Blank.xlsx
+++ b/Tools/Clerk Blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114FC856-F865-4F70-8511-5924DB46DF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB8A2B7-4EAF-4AF4-8E3D-16AE635CD54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Staged Loaded Average</t>
   </si>
@@ -148,51 +148,9 @@
     <t xml:space="preserve">Lane </t>
   </si>
   <si>
-    <t>RM-TRURO-GB-H2</t>
-  </si>
-  <si>
-    <t>RM-SWANSEA-GB-H2</t>
-  </si>
-  <si>
-    <t>RM-PLYMOUTH-GB-H2</t>
-  </si>
-  <si>
-    <t>15/16</t>
-  </si>
-  <si>
-    <t>RM-EXETER-GB-H2</t>
-  </si>
-  <si>
-    <t>16/17</t>
-  </si>
-  <si>
-    <t>RM-CARDIFF-GB-H2</t>
-  </si>
-  <si>
-    <t>17/18</t>
-  </si>
-  <si>
-    <t>RM-BRISTOL2-GB-H2</t>
-  </si>
-  <si>
-    <t>RM-BRISTOL-GB-H1</t>
-  </si>
-  <si>
-    <t>AIR-BRS2-EMSA</t>
-  </si>
-  <si>
-    <t>DPD-BURBAGE-GB-H1</t>
-  </si>
-  <si>
     <t>DXN1-ND</t>
   </si>
   <si>
-    <t>DWR1-DCE1-ND-MR</t>
-  </si>
-  <si>
-    <t>DHA1-DCR2-ND-MR</t>
-  </si>
-  <si>
     <t>DBS3-ND</t>
   </si>
   <si>
@@ -202,24 +160,12 @@
     <t>DST1-ND</t>
   </si>
   <si>
-    <t>LMC</t>
-  </si>
-  <si>
     <t>DXE1-ND</t>
   </si>
   <si>
-    <t>DBI2-DBI7-MR-ND</t>
-  </si>
-  <si>
-    <t>DXM2-DPR1-MR-ND</t>
-  </si>
-  <si>
     <t>DOX2-ND</t>
   </si>
   <si>
-    <t>DRG2-DXW2-MR-ND</t>
-  </si>
-  <si>
     <t>DBI5-ND</t>
   </si>
   <si>
@@ -227,13 +173,85 @@
   </si>
   <si>
     <t>DPE2-ND</t>
+  </si>
+  <si>
+    <t>51/52</t>
+  </si>
+  <si>
+    <t>JP Carts</t>
+  </si>
+  <si>
+    <t>42/43</t>
+  </si>
+  <si>
+    <t>DXW2-MR</t>
+  </si>
+  <si>
+    <t>DRG2-MR</t>
+  </si>
+  <si>
+    <t>DPR1-MR</t>
+  </si>
+  <si>
+    <t>DXM2-MR</t>
+  </si>
+  <si>
+    <t>DBI7-MR</t>
+  </si>
+  <si>
+    <t>DBI2-MR</t>
+  </si>
+  <si>
+    <t>SWANSEA</t>
+  </si>
+  <si>
+    <t>PLYMOUTH</t>
+  </si>
+  <si>
+    <t>EXETER</t>
+  </si>
+  <si>
+    <t>CARDIFF</t>
+  </si>
+  <si>
+    <t>BRISTOL2</t>
+  </si>
+  <si>
+    <t>RM-BRISTOL-H1</t>
+  </si>
+  <si>
+    <t>BFSA</t>
+  </si>
+  <si>
+    <t>DPD</t>
+  </si>
+  <si>
+    <t>DWR1-MR</t>
+  </si>
+  <si>
+    <t>DCE1-MR</t>
+  </si>
+  <si>
+    <t>30/31</t>
+  </si>
+  <si>
+    <t>DCR2-MR</t>
+  </si>
+  <si>
+    <t>DHA1-MR</t>
+  </si>
+  <si>
+    <t>DBI4-ND</t>
+  </si>
+  <si>
+    <t>RM-BRISTOL-HV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,19 +268,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -276,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -570,13 +581,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -597,19 +605,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -895,7 +901,7 @@
   <dimension ref="A1:AQ32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB29" sqref="BB29"/>
+      <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,29 +935,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="E1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="I1" s="20" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="22"/>
-      <c r="M1" s="20" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="25"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="24"/>
       <c r="T1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1036,20 +1042,23 @@
       <c r="AD3" s="7"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="7"/>
-      <c r="AI3" s="30" t="s">
+      <c r="AI3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="AJ3" s="30" t="s">
+      <c r="AJ3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="30"/>
-      <c r="AO3" s="28" t="s">
+      <c r="AK3" s="17"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AP3" s="28" t="s">
+      <c r="AP3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AQ3" s="28"/>
+      <c r="AQ3" s="17"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1077,23 +1086,26 @@
       <c r="AD4" s="7"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="7"/>
-      <c r="AI4" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ4" s="29">
-        <v>14</v>
-      </c>
-      <c r="AK4" s="18">
+      <c r="AI4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ4" s="25">
+        <v>16</v>
+      </c>
+      <c r="AK4" s="25">
         <v>2</v>
       </c>
-      <c r="AO4" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP4" s="29">
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP4" s="26">
         <v>39</v>
       </c>
-      <c r="AQ4" s="17">
-        <v>2</v>
+      <c r="AQ4" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1122,22 +1134,25 @@
       <c r="AD5" s="7"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="7"/>
-      <c r="AI5" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ5" s="29">
-        <v>15</v>
-      </c>
-      <c r="AK5" s="17">
+      <c r="AI5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ5" s="26">
+        <v>16</v>
+      </c>
+      <c r="AK5" s="26">
         <v>2</v>
       </c>
-      <c r="AO5" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP5" s="29">
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="27"/>
+      <c r="AO5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP5" s="26">
         <v>39</v>
       </c>
-      <c r="AQ5" s="17">
+      <c r="AQ5" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1167,23 +1182,26 @@
       <c r="AD6" s="7"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="7"/>
-      <c r="AI6" s="29" t="s">
+      <c r="AI6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ6" s="26">
+        <v>17</v>
+      </c>
+      <c r="AK6" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP6" s="26">
         <v>39</v>
       </c>
-      <c r="AJ6" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK6" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO6" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP6" s="29">
-        <v>40</v>
-      </c>
-      <c r="AQ6" s="17">
-        <v>2</v>
+      <c r="AQ6" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
@@ -1212,23 +1230,26 @@
       <c r="AD7" s="7"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
-      <c r="AI7" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ7" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK7" s="17">
+      <c r="AI7" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ7" s="26">
+        <v>18</v>
+      </c>
+      <c r="AK7" s="26">
         <v>2</v>
       </c>
-      <c r="AO7" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP7" s="29">
-        <v>41</v>
-      </c>
-      <c r="AQ7" s="17">
-        <v>2</v>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP7" s="26">
+        <v>40</v>
+      </c>
+      <c r="AQ7" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
@@ -1257,23 +1278,26 @@
       <c r="AD8" s="7"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="7"/>
-      <c r="AI8" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ8" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK8" s="17">
+      <c r="AI8" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ8" s="26">
+        <v>18</v>
+      </c>
+      <c r="AK8" s="26">
         <v>2</v>
       </c>
-      <c r="AO8" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP8" s="29">
-        <v>41</v>
-      </c>
-      <c r="AQ8" s="17">
-        <v>2</v>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP8" s="26">
+        <v>40</v>
+      </c>
+      <c r="AQ8" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
@@ -1302,23 +1326,26 @@
       <c r="AD9" s="7"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="7"/>
-      <c r="AI9" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ9" s="29">
-        <v>18</v>
-      </c>
-      <c r="AK9" s="17">
+      <c r="AI9" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ9" s="26">
+        <v>23</v>
+      </c>
+      <c r="AK9" s="26">
         <v>3</v>
       </c>
-      <c r="AO9" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP9" s="29">
-        <v>42</v>
-      </c>
-      <c r="AQ9" s="17">
-        <v>1</v>
+      <c r="AL9" s="27"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP9" s="26">
+        <v>40</v>
+      </c>
+      <c r="AQ9" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1347,23 +1374,26 @@
       <c r="AD10" s="7"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="7"/>
-      <c r="AI10" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ10" s="29">
+      <c r="AI10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ10" s="26">
         <v>23</v>
       </c>
-      <c r="AK10" s="17">
+      <c r="AK10" s="26">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="27"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP10" s="26">
+        <v>41</v>
+      </c>
+      <c r="AQ10" s="26">
         <v>2</v>
-      </c>
-      <c r="AO10" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP10" s="29">
-        <v>42</v>
-      </c>
-      <c r="AQ10" s="17">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
@@ -1392,23 +1422,26 @@
       <c r="AD11" s="7"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="7"/>
-      <c r="AI11" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ11" s="29">
-        <v>23</v>
-      </c>
-      <c r="AK11" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO11" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP11" s="29">
-        <v>43</v>
-      </c>
-      <c r="AQ11" s="17">
+      <c r="AI11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ11" s="26">
+        <v>24</v>
+      </c>
+      <c r="AK11" s="26">
         <v>2</v>
+      </c>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP11" s="26">
+        <v>42</v>
+      </c>
+      <c r="AQ11" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
@@ -1437,22 +1470,25 @@
       <c r="AD12" s="7"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="7"/>
-      <c r="AI12" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ12" s="29">
+      <c r="AI12" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ12" s="26">
         <v>24</v>
       </c>
-      <c r="AK12" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP12" s="29">
-        <v>43</v>
-      </c>
-      <c r="AQ12" s="17">
+      <c r="AK12" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL12" s="27"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP12" s="26">
+        <v>42</v>
+      </c>
+      <c r="AQ12" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1482,23 +1518,26 @@
       <c r="AD13" s="7"/>
       <c r="AF13" s="6"/>
       <c r="AG13" s="7"/>
-      <c r="AI13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ13" s="29">
-        <v>24</v>
-      </c>
-      <c r="AK13" s="17">
+      <c r="AI13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ13" s="26">
+        <v>25</v>
+      </c>
+      <c r="AK13" s="26">
         <v>4</v>
       </c>
-      <c r="AO13" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP13" s="29">
-        <v>44</v>
-      </c>
-      <c r="AQ13" s="17">
-        <v>1</v>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP13" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ13" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
@@ -1527,23 +1566,26 @@
       <c r="AD14" s="7"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="7"/>
-      <c r="AI14" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ14" s="29">
-        <v>25</v>
-      </c>
-      <c r="AK14" s="17">
+      <c r="AI14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ14" s="26">
+        <v>26</v>
+      </c>
+      <c r="AK14" s="26">
         <v>4</v>
       </c>
-      <c r="AO14" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP14" s="29">
-        <v>44</v>
-      </c>
-      <c r="AQ14" s="17">
-        <v>2</v>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP14" s="26">
+        <v>43</v>
+      </c>
+      <c r="AQ14" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
@@ -1572,22 +1614,25 @@
       <c r="AD15" s="7"/>
       <c r="AF15" s="6"/>
       <c r="AG15" s="7"/>
-      <c r="AI15" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ15" s="29">
-        <v>26</v>
-      </c>
-      <c r="AK15" s="17">
+      <c r="AI15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ15" s="26">
+        <v>27</v>
+      </c>
+      <c r="AK15" s="26">
         <v>4</v>
       </c>
-      <c r="AO15" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP15" s="29">
-        <v>45</v>
-      </c>
-      <c r="AQ15" s="17">
+      <c r="AL15" s="27"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
+      <c r="AO15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP15" s="26">
+        <v>43</v>
+      </c>
+      <c r="AQ15" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1617,22 +1662,25 @@
       <c r="AD16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="7"/>
-      <c r="AI16" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ16" s="29">
-        <v>27</v>
-      </c>
-      <c r="AK16" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO16" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP16" s="29">
-        <v>45</v>
-      </c>
-      <c r="AQ16" s="17">
+      <c r="AI16" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ16" s="26">
+        <v>28</v>
+      </c>
+      <c r="AK16" s="26">
+        <v>4</v>
+      </c>
+      <c r="AL16" s="27"/>
+      <c r="AM16" s="27"/>
+      <c r="AN16" s="27"/>
+      <c r="AO16" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP16" s="26">
+        <v>44</v>
+      </c>
+      <c r="AQ16" s="26">
         <v>2</v>
       </c>
     </row>
@@ -1662,22 +1710,25 @@
       <c r="AD17" s="7"/>
       <c r="AF17" s="6"/>
       <c r="AG17" s="7"/>
-      <c r="AI17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ17" s="29">
+      <c r="AI17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ17" s="26">
+        <v>29</v>
+      </c>
+      <c r="AK17" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL17" s="27"/>
+      <c r="AM17" s="27"/>
+      <c r="AN17" s="27"/>
+      <c r="AO17" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AK17" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO17" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP17" s="29">
-        <v>46</v>
-      </c>
-      <c r="AQ17" s="17">
+      <c r="AP17" s="26">
+        <v>44</v>
+      </c>
+      <c r="AQ17" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1707,23 +1758,26 @@
       <c r="AD18" s="7"/>
       <c r="AF18" s="6"/>
       <c r="AG18" s="7"/>
-      <c r="AI18" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ18" s="29">
+      <c r="AI18" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ18" s="26">
         <v>29</v>
       </c>
-      <c r="AK18" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO18" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP18" s="29">
-        <v>46</v>
-      </c>
-      <c r="AQ18" s="17">
-        <v>1</v>
+      <c r="AK18" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL18" s="27"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="27"/>
+      <c r="AO18" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP18" s="26">
+        <v>45</v>
+      </c>
+      <c r="AQ18" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
@@ -1752,22 +1806,25 @@
       <c r="AD19" s="7"/>
       <c r="AF19" s="6"/>
       <c r="AG19" s="7"/>
-      <c r="AI19" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ19" s="29">
+      <c r="AI19" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ19" s="26">
         <v>30</v>
       </c>
-      <c r="AK19" s="17">
-        <v>5</v>
-      </c>
-      <c r="AO19" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP19" s="29">
-        <v>47</v>
-      </c>
-      <c r="AQ19" s="17">
+      <c r="AK19" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL19" s="27"/>
+      <c r="AM19" s="27"/>
+      <c r="AN19" s="27"/>
+      <c r="AO19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP19" s="26">
+        <v>45</v>
+      </c>
+      <c r="AQ19" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1797,22 +1854,25 @@
       <c r="AD20" s="7"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
-      <c r="AI20" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ20" s="29">
-        <v>31</v>
-      </c>
-      <c r="AK20" s="17">
-        <v>4</v>
-      </c>
-      <c r="AO20" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="AP20" s="29">
+      <c r="AI20" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AQ20" s="17">
+      <c r="AJ20" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK20" s="26">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="27"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
+      <c r="AO20" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP20" s="26">
+        <v>46</v>
+      </c>
+      <c r="AQ20" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1842,22 +1902,25 @@
       <c r="AD21" s="7"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="7"/>
-      <c r="AI21" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ21" s="29">
-        <v>32</v>
-      </c>
-      <c r="AK21" s="17">
+      <c r="AI21" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ21" s="26">
+        <v>31</v>
+      </c>
+      <c r="AK21" s="26">
         <v>4</v>
       </c>
-      <c r="AO21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP21" s="29">
-        <v>48</v>
-      </c>
-      <c r="AQ21" s="17">
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="27"/>
+      <c r="AO21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP21" s="26">
+        <v>46</v>
+      </c>
+      <c r="AQ21" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1887,22 +1950,25 @@
       <c r="AD22" s="7"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="7"/>
-      <c r="AI22" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ22" s="29">
-        <v>33</v>
-      </c>
-      <c r="AK22" s="17">
+      <c r="AI22" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ22" s="26">
+        <v>32</v>
+      </c>
+      <c r="AK22" s="26">
         <v>4</v>
       </c>
-      <c r="AO22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP22" s="29">
-        <v>49</v>
-      </c>
-      <c r="AQ22" s="19">
+      <c r="AL22" s="27"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
+      <c r="AO22" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP22" s="26">
+        <v>46</v>
+      </c>
+      <c r="AQ22" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1932,22 +1998,25 @@
       <c r="AD23" s="7"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="7"/>
-      <c r="AI23" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ23" s="29">
-        <v>34</v>
-      </c>
-      <c r="AK23" s="17">
-        <v>6</v>
-      </c>
-      <c r="AO23" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP23" s="29">
-        <v>50</v>
-      </c>
-      <c r="AQ23" s="19">
+      <c r="AI23" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ23" s="26">
+        <v>33</v>
+      </c>
+      <c r="AK23" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL23" s="27"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="27"/>
+      <c r="AO23" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP23" s="26">
+        <v>47</v>
+      </c>
+      <c r="AQ23" s="26">
         <v>2</v>
       </c>
     </row>
@@ -1977,23 +2046,26 @@
       <c r="AD24" s="7"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="7"/>
-      <c r="AI24" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ24" s="29">
-        <v>35</v>
-      </c>
-      <c r="AK24" s="17">
+      <c r="AI24" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ24" s="26">
+        <v>33</v>
+      </c>
+      <c r="AK24" s="26">
         <v>2</v>
       </c>
-      <c r="AO24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP24" s="29">
-        <v>50</v>
-      </c>
-      <c r="AQ24" s="19">
-        <v>3</v>
+      <c r="AL24" s="27"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="27"/>
+      <c r="AO24" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP24" s="26">
+        <v>47</v>
+      </c>
+      <c r="AQ24" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
@@ -2022,22 +2094,25 @@
       <c r="AD25" s="7"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
-      <c r="AI25" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ25" s="29">
-        <v>36</v>
-      </c>
-      <c r="AK25" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO25" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP25" s="29">
-        <v>51</v>
-      </c>
-      <c r="AQ25" s="19">
+      <c r="AI25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ25" s="26">
+        <v>34</v>
+      </c>
+      <c r="AK25" s="26">
+        <v>5</v>
+      </c>
+      <c r="AL25" s="27"/>
+      <c r="AM25" s="27"/>
+      <c r="AN25" s="27"/>
+      <c r="AO25" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP25" s="26">
+        <v>49</v>
+      </c>
+      <c r="AQ25" s="26">
         <v>1</v>
       </c>
     </row>
@@ -2067,23 +2142,26 @@
       <c r="AD26" s="7"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="7"/>
-      <c r="AI26" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ26" s="29">
-        <v>37</v>
-      </c>
-      <c r="AK26" s="17">
+      <c r="AI26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ26" s="26">
+        <v>35</v>
+      </c>
+      <c r="AK26" s="26">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP26" s="26">
+        <v>49</v>
+      </c>
+      <c r="AQ26" s="26">
         <v>2</v>
-      </c>
-      <c r="AO26" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP26" s="29">
-        <v>51</v>
-      </c>
-      <c r="AQ26" s="19">
-        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -2112,23 +2190,26 @@
       <c r="AD27" s="7"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="7"/>
-      <c r="AI27" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ27" s="29">
+      <c r="AI27" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AK27" s="17">
+      <c r="AJ27" s="26">
+        <v>35</v>
+      </c>
+      <c r="AK27" s="26">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="27"/>
+      <c r="AM27" s="27"/>
+      <c r="AN27" s="27"/>
+      <c r="AO27" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP27" s="26">
+        <v>50</v>
+      </c>
+      <c r="AQ27" s="26">
         <v>3</v>
-      </c>
-      <c r="AO27" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="AP27" s="29">
-        <v>52</v>
-      </c>
-      <c r="AQ27" s="19">
-        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
@@ -2157,6 +2238,27 @@
       <c r="AD28" s="7"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="7"/>
+      <c r="AI28" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ28" s="26">
+        <v>35</v>
+      </c>
+      <c r="AK28" s="26">
+        <v>1</v>
+      </c>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
+      <c r="AO28" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP28" s="26">
+        <v>51</v>
+      </c>
+      <c r="AQ28" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
@@ -2184,9 +2286,27 @@
       <c r="AD29" s="7"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="7"/>
-      <c r="AO29" s="26"/>
-      <c r="AP29" s="27"/>
-      <c r="AQ29" s="26"/>
+      <c r="AI29" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ29" s="26">
+        <v>36</v>
+      </c>
+      <c r="AK29" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
+      <c r="AO29" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP29" s="18">
+        <v>51</v>
+      </c>
+      <c r="AQ29" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
@@ -2214,6 +2334,27 @@
       <c r="AD30" s="7"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="7"/>
+      <c r="AI30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ30" s="26">
+        <v>36</v>
+      </c>
+      <c r="AK30" s="26">
+        <v>2</v>
+      </c>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="27"/>
+      <c r="AO30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP30" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ30" s="26">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
@@ -2241,6 +2382,27 @@
       <c r="AD31" s="7"/>
       <c r="AF31" s="6"/>
       <c r="AG31" s="7"/>
+      <c r="AI31" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ31" s="26">
+        <v>37</v>
+      </c>
+      <c r="AK31" s="26">
+        <v>3</v>
+      </c>
+      <c r="AL31" s="27"/>
+      <c r="AM31" s="27"/>
+      <c r="AN31" s="27"/>
+      <c r="AO31" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP31" s="18">
+        <v>52</v>
+      </c>
+      <c r="AQ31" s="29">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>

</xml_diff>

<commit_message>
updated clerk blank and capacity check
</commit_message>
<xml_diff>
--- a/Tools/Clerk Blank.xlsx
+++ b/Tools/Clerk Blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gardsimo\Downloads\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36486E5-C01C-47E3-9B5C-2FDA6499563A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BECAA9-F6F4-4110-BC43-D4611705E0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,20 +220,20 @@
     <t>DCR2-ND</t>
   </si>
   <si>
-    <t>DCR3-MR</t>
-  </si>
-  <si>
     <t>DBI5-MR</t>
   </si>
   <si>
     <t>DXM4-ND</t>
+  </si>
+  <si>
+    <t>DCR3-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,13 +263,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -296,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -540,6 +533,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -595,6 +599,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -613,10 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -902,7 +906,7 @@
   <dimension ref="A1:AQ32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU15" sqref="AU15"/>
+      <selection activeCell="AU13" sqref="AU13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,29 +940,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="E1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
-      <c r="I1" s="24" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="I1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
-      <c r="M1" s="24" t="s">
+      <c r="J1" s="26"/>
+      <c r="K1" s="27"/>
+      <c r="M1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="29"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="30"/>
       <c r="T1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1436,10 +1440,10 @@
       <c r="AM11" s="21"/>
       <c r="AN11" s="21"/>
       <c r="AO11" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP11" s="20">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AQ11" s="20">
         <v>2</v>
@@ -1484,10 +1488,10 @@
       <c r="AM12" s="21"/>
       <c r="AN12" s="21"/>
       <c r="AO12" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP12" s="20">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="AP12" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="AQ12" s="20">
         <v>2</v>
@@ -1531,14 +1535,14 @@
       <c r="AL13" s="21"/>
       <c r="AM13" s="21"/>
       <c r="AN13" s="21"/>
-      <c r="AO13" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP13" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ13" s="20">
-        <v>2</v>
+      <c r="AO13" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP13" s="31">
+        <v>43</v>
+      </c>
+      <c r="AQ13" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
@@ -1856,7 +1860,7 @@
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
       <c r="AI20" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AJ20" s="20">
         <v>30</v>
@@ -2095,10 +2099,10 @@
       <c r="AD25" s="7"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
-      <c r="AI25" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ25" s="31">
+      <c r="AI25" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ25" s="24">
         <v>33</v>
       </c>
       <c r="AK25" s="20">

</xml_diff>